<commit_message>
added components to xls
</commit_message>
<xml_diff>
--- a/CloudKitchen-artifacts/Routes.xlsx
+++ b/CloudKitchen-artifacts/Routes.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Admin" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="106">
   <si>
     <t xml:space="preserve">Operation</t>
   </si>
@@ -37,6 +37,9 @@
     <t xml:space="preserve">function</t>
   </si>
   <si>
+    <t xml:space="preserve">Components</t>
+  </si>
+  <si>
     <t xml:space="preserve">Login </t>
   </si>
   <si>
@@ -49,6 +52,9 @@
     <t xml:space="preserve">for admin to login</t>
   </si>
   <si>
+    <t xml:space="preserve">Admin-Login</t>
+  </si>
+  <si>
     <t xml:space="preserve">Dashboard</t>
   </si>
   <si>
@@ -58,18 +64,27 @@
     <t xml:space="preserve">to fetch all orders.</t>
   </si>
   <si>
+    <t xml:space="preserve">Admin-view-orders</t>
+  </si>
+  <si>
     <t xml:space="preserve">/viewRestaurants</t>
   </si>
   <si>
     <t xml:space="preserve">to fetch all restaurants.</t>
   </si>
   <si>
+    <t xml:space="preserve">Admin-view-restaurant</t>
+  </si>
+  <si>
     <t xml:space="preserve">/viewCustomers</t>
   </si>
   <si>
     <t xml:space="preserve">to fetch all customers.</t>
   </si>
   <si>
+    <t xml:space="preserve">Admin-view-delivery-persons</t>
+  </si>
+  <si>
     <t xml:space="preserve">/viewDeliveryPersons</t>
   </si>
   <si>
@@ -118,18 +133,27 @@
     <t xml:space="preserve">delete delivery person.</t>
   </si>
   <si>
+    <t xml:space="preserve">*yellow marked component will be the component that will load first after login</t>
+  </si>
+  <si>
     <t xml:space="preserve">Request Type</t>
   </si>
   <si>
     <t xml:space="preserve">Function</t>
   </si>
   <si>
+    <t xml:space="preserve">Component</t>
+  </si>
+  <si>
     <t xml:space="preserve">Login</t>
   </si>
   <si>
     <t xml:space="preserve">for restaurants to login.</t>
   </si>
   <si>
+    <t xml:space="preserve">Restaurant-login</t>
+  </si>
+  <si>
     <t xml:space="preserve">Register</t>
   </si>
   <si>
@@ -142,6 +166,9 @@
     <t xml:space="preserve">for restaurants to register.</t>
   </si>
   <si>
+    <t xml:space="preserve">Restaurant-register</t>
+  </si>
+  <si>
     <t xml:space="preserve">Food</t>
   </si>
   <si>
@@ -151,6 +178,9 @@
     <t xml:space="preserve">adds a food to the restaurants menu.</t>
   </si>
   <si>
+    <t xml:space="preserve">Restaurant-add-food</t>
+  </si>
+  <si>
     <t xml:space="preserve">/updateFood</t>
   </si>
   <si>
@@ -166,30 +196,48 @@
     <t xml:space="preserve">to update restaurants profile</t>
   </si>
   <si>
+    <t xml:space="preserve">Restaurant-update-profile</t>
+  </si>
+  <si>
     <t xml:space="preserve">/updateAmbience</t>
   </si>
   <si>
     <t xml:space="preserve">to upload ambience photos of restaurant.</t>
   </si>
   <si>
+    <t xml:space="preserve">Restaurant-ambient-photos</t>
+  </si>
+  <si>
     <t xml:space="preserve">/getOrders</t>
   </si>
   <si>
     <t xml:space="preserve">to display orders for that restaurant.</t>
   </si>
   <si>
+    <t xml:space="preserve">Restaurant-view-orders</t>
+  </si>
+  <si>
     <t xml:space="preserve">to change the state of orders.</t>
   </si>
   <si>
     <t xml:space="preserve">for dp to login.</t>
   </si>
   <si>
+    <t xml:space="preserve">Delivery-person-login</t>
+  </si>
+  <si>
     <t xml:space="preserve">for dp to register.</t>
   </si>
   <si>
+    <t xml:space="preserve">Delivery-person-register</t>
+  </si>
+  <si>
     <t xml:space="preserve">to display orders that have pending state.</t>
   </si>
   <si>
+    <t xml:space="preserve">Delivery-person-view-orders</t>
+  </si>
+  <si>
     <t xml:space="preserve">/pickedOrder</t>
   </si>
   <si>
@@ -205,6 +253,9 @@
     <t xml:space="preserve">to display all penalties.</t>
   </si>
   <si>
+    <t xml:space="preserve">Delivery-person-view-penalties</t>
+  </si>
+  <si>
     <t xml:space="preserve">/payPenalty</t>
   </si>
   <si>
@@ -214,21 +265,36 @@
     <t xml:space="preserve">to update dp profile.</t>
   </si>
   <si>
+    <t xml:space="preserve">Delivery-person-update-profile</t>
+  </si>
+  <si>
     <t xml:space="preserve">for customer to login.</t>
   </si>
   <si>
+    <t xml:space="preserve">Customer-login</t>
+  </si>
+  <si>
     <t xml:space="preserve">for customer to register. </t>
   </si>
   <si>
+    <t xml:space="preserve">Customer-register</t>
+  </si>
+  <si>
     <t xml:space="preserve">to update customer profile.</t>
   </si>
   <si>
+    <t xml:space="preserve">Customer-update-profile</t>
+  </si>
+  <si>
     <t xml:space="preserve">View Restaurants</t>
   </si>
   <si>
     <t xml:space="preserve">/viewRestaurant</t>
   </si>
   <si>
+    <t xml:space="preserve">Customer-view-restaurant</t>
+  </si>
+  <si>
     <t xml:space="preserve">/filterRestaurant</t>
   </si>
   <si>
@@ -241,12 +307,18 @@
     <t xml:space="preserve">to fetch all details of restaurant with ambient images and foods.</t>
   </si>
   <si>
+    <t xml:space="preserve">Customer-view-restaurant-detail</t>
+  </si>
+  <si>
     <t xml:space="preserve">View Orders</t>
   </si>
   <si>
     <t xml:space="preserve">to fetch all orders by that customer.</t>
   </si>
   <si>
+    <t xml:space="preserve">Customer-view-orders</t>
+  </si>
+  <si>
     <t xml:space="preserve">/cancelOrders</t>
   </si>
   <si>
@@ -260,6 +332,9 @@
   </si>
   <si>
     <t xml:space="preserve">to place the order for that customer.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Customer-place-order</t>
   </si>
   <si>
     <t xml:space="preserve">/updateAddress</t>
@@ -275,11 +350,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -301,12 +377,14 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -314,9 +392,22 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -327,6 +418,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF81D41A"/>
         <bgColor rgb="FF969696"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF38"/>
       </patternFill>
     </fill>
     <fill>
@@ -388,7 +485,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="23">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -421,11 +518,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -437,15 +542,19 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -457,11 +566,15 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -481,7 +594,7 @@
       <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF38"/>
+      <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
@@ -502,7 +615,7 @@
       <rgbColor rgb="FFCCCCFF"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFFFF38"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF800000"/>
@@ -542,18 +655,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="22.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="22.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="34.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="26.62"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -569,134 +683,161 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>14</v>
+        <v>18</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>18</v>
+        <v>22</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>23</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>22</v>
+        <v>26</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>27</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>22</v>
+        <v>30</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>27</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>22</v>
+        <v>33</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>27</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>30</v>
-      </c>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E11" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E11:I11"/>
+  </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -712,18 +853,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="4" width="17.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="28.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="23.08"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -731,131 +873,164 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>32</v>
+        <v>38</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>34</v>
+        <v>41</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>36</v>
+        <v>43</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>44</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" s="11" customFormat="true" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>41</v>
+        <v>46</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" s="13" customFormat="true" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>18</v>
+        <v>48</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>23</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>18</v>
+        <v>54</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>23</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="7" s="11" customFormat="true" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="B7" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="8" s="11" customFormat="true" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>50</v>
+        <v>56</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" s="13" customFormat="true" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" s="13" customFormat="true" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>18</v>
+        <v>22</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>23</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>51</v>
-      </c>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E10" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E10:I10"/>
+  </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -868,18 +1043,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
+      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="4" width="22.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="22.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="4" width="22.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="22.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="23.62"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -887,117 +1063,147 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>32</v>
+        <v>38</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>52</v>
+        <v>65</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3" s="14" t="s">
-        <v>36</v>
+        <v>43</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>44</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="4" s="17" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>54</v>
+        <v>67</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" s="21" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="E4" s="20" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>18</v>
+        <v>10</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>23</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>56</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>57</v>
+        <v>73</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>58</v>
+        <v>74</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>59</v>
+        <v>75</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>18</v>
+        <v>73</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>23</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>60</v>
+        <v>77</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>61</v>
+        <v>78</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>18</v>
+        <v>54</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>23</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>62</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E9" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E9:I9"/>
+  </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1010,18 +1216,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="4" width="19.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="27.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="23.08"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1029,159 +1236,195 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>32</v>
+        <v>38</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>63</v>
+        <v>81</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3" s="14" t="s">
-        <v>36</v>
+        <v>43</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>44</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>64</v>
+        <v>83</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>18</v>
+        <v>54</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>23</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>65</v>
+        <v>85</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>66</v>
+        <v>87</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>67</v>
+        <v>88</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" s="11" customFormat="true" ht="26.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="B6" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="7" s="11" customFormat="true" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="B7" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="8" s="11" customFormat="true" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="B8" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>73</v>
+        <v>15</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6" s="13" customFormat="true" ht="26.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="7" s="13" customFormat="true" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="8" s="13" customFormat="true" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>18</v>
+        <v>95</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>23</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>74</v>
+        <v>98</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="10" s="11" customFormat="true" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="B10" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>78</v>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="10" s="13" customFormat="true" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="B10" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>18</v>
+        <v>100</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>23</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>79</v>
+        <v>104</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>80</v>
-      </c>
+        <v>105</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E12" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E12:I12"/>
+  </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
Added Customer Routes - PUT
</commit_message>
<xml_diff>
--- a/CloudKitchen-artifacts/Routes.xlsx
+++ b/CloudKitchen-artifacts/Routes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Project Artifacts- Project Cloud Kitchen\CloudKitchen\CloudKitchen-artifacts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D430E408-DB22-4C66-AFC0-3DF754AA389F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F832F5B-9FA0-475F-B86F-9A67A9053A9E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19260" yWindow="2340" windowWidth="16200" windowHeight="9360" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Admin" sheetId="1" r:id="rId1"/>
@@ -394,7 +394,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -443,12 +443,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -462,7 +456,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -509,13 +503,12 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -901,7 +894,7 @@
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -937,7 +930,7 @@
       <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="24" t="s">
+      <c r="C2" s="22" t="s">
         <v>7</v>
       </c>
       <c r="D2" t="s">
@@ -954,7 +947,7 @@
       <c r="B3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="24" t="s">
+      <c r="C3" s="22" t="s">
         <v>11</v>
       </c>
       <c r="D3" t="s">
@@ -971,7 +964,7 @@
       <c r="B4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="24" t="s">
+      <c r="C4" s="22" t="s">
         <v>14</v>
       </c>
       <c r="D4" t="s">
@@ -988,7 +981,7 @@
       <c r="B5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="24" t="s">
+      <c r="C5" s="22" t="s">
         <v>17</v>
       </c>
       <c r="D5" t="s">
@@ -1005,7 +998,7 @@
       <c r="B6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="24" t="s">
+      <c r="C6" s="22" t="s">
         <v>20</v>
       </c>
       <c r="D6" t="s">
@@ -1069,13 +1062,13 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="E11" s="22" t="s">
+      <c r="E11" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="F11" s="22"/>
-      <c r="G11" s="22"/>
-      <c r="H11" s="22"/>
-      <c r="I11" s="22"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1255,13 +1248,13 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="E10" s="22" t="s">
+      <c r="E10" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="F10" s="22"/>
-      <c r="G10" s="22"/>
-      <c r="H10" s="22"/>
-      <c r="I10" s="22"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1424,13 +1417,13 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="E9" s="22" t="s">
+      <c r="E9" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="F9" s="22"/>
-      <c r="G9" s="22"/>
-      <c r="H9" s="22"/>
-      <c r="I9" s="22"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="24"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1450,7 +1443,7 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1486,7 +1479,7 @@
       <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="24" t="s">
+      <c r="C2" s="22" t="s">
         <v>7</v>
       </c>
       <c r="D2" t="s">
@@ -1503,7 +1496,7 @@
       <c r="B3" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="C3" s="24" t="s">
+      <c r="C3" s="22" t="s">
         <v>45</v>
       </c>
       <c r="D3" t="s">
@@ -1520,7 +1513,7 @@
       <c r="B4" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="26" t="s">
+      <c r="C4" s="22" t="s">
         <v>55</v>
       </c>
       <c r="D4" t="s">
@@ -1537,7 +1530,7 @@
       <c r="B5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="24" t="s">
+      <c r="C5" s="22" t="s">
         <v>88</v>
       </c>
       <c r="D5" t="s">
@@ -1554,7 +1547,7 @@
       <c r="B6" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="25" t="s">
+      <c r="C6" s="23" t="s">
         <v>90</v>
       </c>
       <c r="D6" s="12" t="s">
@@ -1568,7 +1561,7 @@
       <c r="B7" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="25" t="s">
+      <c r="C7" s="23" t="s">
         <v>92</v>
       </c>
       <c r="D7" s="12" t="s">
@@ -1585,7 +1578,7 @@
       <c r="B8" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="25" t="s">
+      <c r="C8" s="23" t="s">
         <v>11</v>
       </c>
       <c r="D8" s="12" t="s">
@@ -1602,7 +1595,7 @@
       <c r="B9" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="22" t="s">
         <v>98</v>
       </c>
       <c r="D9" t="s">
@@ -1633,7 +1626,7 @@
       <c r="B11" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="22" t="s">
         <v>104</v>
       </c>
       <c r="D11" t="s">
@@ -1641,13 +1634,13 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="E12" s="23" t="s">
+      <c r="E12" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="F12" s="23"/>
-      <c r="G12" s="23"/>
-      <c r="H12" s="23"/>
-      <c r="I12" s="23"/>
+      <c r="F12" s="25"/>
+      <c r="G12" s="25"/>
+      <c r="H12" s="25"/>
+      <c r="I12" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>